<commit_message>
Add Order and OrderLine and Configuration and Notification + Update on diagramme de cas d'utilisation
</commit_message>
<xml_diff>
--- a/Modelisation/Dictionnaire de donnee.xlsx
+++ b/Modelisation/Dictionnaire de donnee.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="10455" windowHeight="5385" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="10455" windowHeight="5325" tabRatio="990" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Societé" sheetId="1" r:id="rId1"/>
@@ -15,14 +15,17 @@
     <sheet name="MaterialCategory" sheetId="6" r:id="rId6"/>
     <sheet name="Emplacement" sheetId="7" r:id="rId7"/>
     <sheet name="Service" sheetId="8" r:id="rId8"/>
+    <sheet name="Configuration" sheetId="9" r:id="rId9"/>
+    <sheet name="Order" sheetId="10" r:id="rId10"/>
+    <sheet name="OrderLine" sheetId="11" r:id="rId11"/>
+    <sheet name="Notification" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="137">
   <si>
     <t>Attributs</t>
   </si>
@@ -320,13 +323,130 @@
   </si>
   <si>
     <t>INN_Number</t>
+  </si>
+  <si>
+    <t>Configuration</t>
+  </si>
+  <si>
+    <t>الاعدادات</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>الاسم</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>الوصف</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>Commande</t>
+  </si>
+  <si>
+    <t>الطلب</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>OrderDate</t>
+  </si>
+  <si>
+    <t>Date Commande</t>
+  </si>
+  <si>
+    <t>تاريخ الطلب</t>
+  </si>
+  <si>
+    <t>DeliveryDateExpected</t>
+  </si>
+  <si>
+    <t>DateLivraisonAttendue</t>
+  </si>
+  <si>
+    <t>تاريخ التوصل المنتظر</t>
+  </si>
+  <si>
+    <t>Provider</t>
+  </si>
+  <si>
+    <t>Fournisseur</t>
+  </si>
+  <si>
+    <t>الموزع</t>
+  </si>
+  <si>
+    <t>OrderLine</t>
+  </si>
+  <si>
+    <t>LigneCommande</t>
+  </si>
+  <si>
+    <t>خط الطلب</t>
+  </si>
+  <si>
+    <t>TVA</t>
+  </si>
+  <si>
+    <t>RisqueDeStock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                RiskOfStock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                TVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                            عتبة المخزون</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                الضريبة</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Quantite</t>
+  </si>
+  <si>
+    <t>الكمية</t>
+  </si>
+  <si>
+    <t>Article</t>
+  </si>
+  <si>
+    <t>تاريخ الانشاء</t>
+  </si>
+  <si>
+    <t>اشعار</t>
+  </si>
+  <si>
+    <t>Notification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                         name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                      Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   Creation date</t>
+  </si>
+  <si>
+    <t>date Creation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,7 +478,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,6 +500,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -483,7 +609,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -582,6 +708,86 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -590,6 +796,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -668,6 +879,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -702,6 +914,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -877,28 +1090,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43" customWidth="1"/>
     <col min="2" max="2" width="43.5703125" customWidth="1"/>
     <col min="3" max="3" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75">
+    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="21"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -909,7 +1122,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -920,7 +1133,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -931,7 +1144,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>52</v>
       </c>
@@ -951,29 +1164,428 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.42578125" customWidth="1"/>
+    <col min="2" max="2" width="36.85546875" customWidth="1"/>
+    <col min="3" max="3" width="52.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" s="46" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="46" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="46" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="55"/>
+      <c r="F6" s="56"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="48" t="s">
+        <v>114</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" s="49"/>
+      <c r="F7" s="50"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="E8" s="49"/>
+      <c r="F8" s="50"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="47" t="s">
+        <v>117</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="47" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="51" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="52"/>
+      <c r="F9" s="53"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.42578125" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="59" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="62" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="62" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="62" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" s="58"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="62" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" s="62" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" s="62" t="s">
+        <v>128</v>
+      </c>
+      <c r="D19" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="55"/>
+      <c r="F19" s="56"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="B20" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="C20" s="61" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="49"/>
+      <c r="F20" s="50"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="62" t="s">
+        <v>104</v>
+      </c>
+      <c r="B21" s="61" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="61" t="s">
+        <v>106</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="49"/>
+      <c r="F21" s="50"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.28515625" customWidth="1"/>
+    <col min="2" max="2" width="50" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="59" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="58" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="57" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" s="58" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="58" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="58" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="58" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="58" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="62" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="57" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" s="58" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="63"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="58"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="58"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="58"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="58"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="58"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="58"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="58"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="58"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="58"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="58"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="58"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="58"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="58"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
     <col min="2" max="2" width="35.140625" customWidth="1"/>
     <col min="3" max="3" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="24"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -984,7 +1596,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>92</v>
       </c>
@@ -995,7 +1607,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1006,7 +1618,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>9</v>
       </c>
@@ -1017,7 +1629,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>48</v>
       </c>
@@ -1033,7 +1645,7 @@
       <c r="E6" s="25"/>
       <c r="F6" s="25"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>90</v>
       </c>
@@ -1060,28 +1672,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.140625" customWidth="1"/>
     <col min="2" max="2" width="34.28515625" customWidth="1"/>
     <col min="3" max="3" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="21"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1092,7 +1704,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -1103,7 +1715,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1114,7 +1726,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -1125,7 +1737,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
@@ -1136,7 +1748,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>13</v>
       </c>
@@ -1147,7 +1759,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
@@ -1158,7 +1770,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
@@ -1169,7 +1781,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -1180,7 +1792,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
@@ -1191,7 +1803,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
@@ -1202,7 +1814,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>19</v>
       </c>
@@ -1213,7 +1825,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>33</v>
       </c>
@@ -1224,7 +1836,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>20</v>
       </c>
@@ -1235,7 +1847,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>73</v>
       </c>
@@ -1251,7 +1863,7 @@
       <c r="E16" s="25"/>
       <c r="F16" s="25"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>48</v>
       </c>
@@ -1267,7 +1879,7 @@
       <c r="E17" s="26"/>
       <c r="F17" s="26"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>79</v>
       </c>
@@ -1283,10 +1895,10 @@
       <c r="E18" s="26"/>
       <c r="F18" s="26"/>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
     </row>
   </sheetData>
@@ -1302,28 +1914,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
     <col min="2" max="2" width="34.140625" customWidth="1"/>
     <col min="3" max="3" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="23"/>
       <c r="C1" s="24"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1334,7 +1946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
@@ -1345,7 +1957,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>22</v>
       </c>
@@ -1356,7 +1968,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>23</v>
       </c>
@@ -1367,7 +1979,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>70</v>
       </c>
@@ -1378,7 +1990,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
     </row>
   </sheetData>
@@ -1390,28 +2002,28 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.140625" customWidth="1"/>
     <col min="2" max="2" width="34.28515625" customWidth="1"/>
     <col min="3" max="3" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="21"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1422,7 +2034,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -1433,7 +2045,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -1444,7 +2056,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -1455,7 +2067,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -1466,7 +2078,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>76</v>
       </c>
@@ -1482,7 +2094,7 @@
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>73</v>
       </c>
@@ -1498,7 +2110,7 @@
       <c r="E8" s="26"/>
       <c r="F8" s="26"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>83</v>
       </c>
@@ -1526,27 +2138,27 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="34.42578125" customWidth="1"/>
     <col min="3" max="3" width="34.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="29"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1557,7 +2169,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -1568,7 +2180,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -1579,7 +2191,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>79</v>
       </c>
@@ -1599,27 +2211,27 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="34.28515625" customWidth="1"/>
     <col min="3" max="3" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="21"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1630,7 +2242,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -1641,7 +2253,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
@@ -1652,7 +2264,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>83</v>
       </c>
@@ -1668,7 +2280,7 @@
       <c r="E5" s="30"/>
       <c r="F5" s="30"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>85</v>
       </c>
@@ -1695,27 +2307,27 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="34.28515625" customWidth="1"/>
     <col min="3" max="3" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="29"/>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1726,7 +2338,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1737,7 +2349,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -1748,7 +2360,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>85</v>
       </c>
@@ -1762,7 +2374,7 @@
       <c r="E5" s="33"/>
       <c r="F5" s="33"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="17"/>
       <c r="B6" s="17"/>
       <c r="C6" s="17"/>
@@ -1778,4 +2390,107 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="A1:C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" customWidth="1"/>
+    <col min="3" max="3" width="44.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="39"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="40"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="42"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="42"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="42"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>